<commit_message>
wrote train validate loop
</commit_message>
<xml_diff>
--- a/cnn/architecture.xlsx
+++ b/cnn/architecture.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\girishng\local\learning\ai_sandbox_2025\cnn\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D7F0868-75C1-4AFA-830E-9392A4E553A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E902AE7-7050-4A07-9AB0-4AB4F6478BA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="16663" windowHeight="9463" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="46">
   <si>
     <t>Stride</t>
   </si>
@@ -106,9 +106,6 @@
     <t>out = ((in + 2p - k) / s) + 1</t>
   </si>
   <si>
-    <t>64 X 64 X 6</t>
-  </si>
-  <si>
     <t>4 x 4</t>
   </si>
   <si>
@@ -139,9 +136,6 @@
     <t>FC2</t>
   </si>
   <si>
-    <t>FC3</t>
-  </si>
-  <si>
     <t>Conv</t>
   </si>
   <si>
@@ -151,19 +145,25 @@
     <t>Dense</t>
   </si>
   <si>
-    <t>linear</t>
-  </si>
-  <si>
-    <t>31 X 31 X 32</t>
-  </si>
-  <si>
-    <t>15 X 15 X 32</t>
-  </si>
-  <si>
-    <t>15 X 15 X 64</t>
-  </si>
-  <si>
-    <t>7 X 7 X 64</t>
+    <t>32 X 15 X 15</t>
+  </si>
+  <si>
+    <t>32 X 31 X 31</t>
+  </si>
+  <si>
+    <t>6 X 64 X 64</t>
+  </si>
+  <si>
+    <t>64 X 15 X 15</t>
+  </si>
+  <si>
+    <t>64 X 7 X 7</t>
+  </si>
+  <si>
+    <t>Flatten</t>
+  </si>
+  <si>
+    <t>sigmoid</t>
   </si>
 </sst>
 </file>
@@ -266,20 +266,26 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -288,12 +294,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -595,357 +595,357 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2" t="s">
+      <c r="B1" s="8"/>
+      <c r="C1" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="E1" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="8" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="2"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="9"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
+      <c r="C2" s="8"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="8"/>
+      <c r="G2" s="8"/>
+      <c r="H2" s="8"/>
       <c r="J2" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A3" s="3"/>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3">
-        <v>1</v>
-      </c>
-      <c r="D3" s="3" t="s">
+      <c r="A3" s="2"/>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2">
+        <v>1</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E3" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="F3" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="G3" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="H3" s="4" t="s">
+      <c r="E3" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H3" s="3" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A4" s="3">
-        <v>1</v>
-      </c>
-      <c r="B4" s="3" t="s">
+      <c r="A4" s="2">
+        <v>1</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="3">
+      <c r="C4" s="2">
         <v>96</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="E4" s="3">
+      <c r="E4" s="2">
         <v>0</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="F4" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="G4" s="3">
+      <c r="G4" s="2">
         <v>4</v>
       </c>
-      <c r="H4" s="3" t="s">
+      <c r="H4" s="2" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A5" s="3"/>
-      <c r="B5" s="3" t="s">
+      <c r="A5" s="2"/>
+      <c r="B5" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="3">
+      <c r="C5" s="2">
         <v>96</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="D5" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="E5" s="3">
+      <c r="E5" s="2">
         <v>0</v>
       </c>
-      <c r="F5" s="3" t="s">
+      <c r="F5" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="G5" s="3">
+      <c r="G5" s="2">
         <v>2</v>
       </c>
-      <c r="H5" s="3" t="s">
+      <c r="H5" s="2" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A6" s="3">
+      <c r="A6" s="2">
         <v>2</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="3">
+      <c r="C6" s="2">
         <v>256</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="D6" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E6" s="3">
+      <c r="E6" s="2">
         <v>0</v>
       </c>
-      <c r="F6" s="3" t="s">
+      <c r="F6" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="G6" s="3">
-        <v>1</v>
-      </c>
-      <c r="H6" s="3" t="s">
+      <c r="G6" s="2">
+        <v>1</v>
+      </c>
+      <c r="H6" s="2" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A7" s="3"/>
-      <c r="B7" s="3" t="s">
+      <c r="A7" s="2"/>
+      <c r="B7" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="3">
+      <c r="C7" s="2">
         <v>256</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="D7" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="E7" s="3">
+      <c r="E7" s="2">
         <v>0</v>
       </c>
-      <c r="F7" s="3" t="s">
+      <c r="F7" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="G7" s="3">
+      <c r="G7" s="2">
         <v>2</v>
       </c>
-      <c r="H7" s="3" t="s">
+      <c r="H7" s="2" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A8" s="3">
+      <c r="A8" s="2">
         <v>3</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="3">
+      <c r="C8" s="2">
         <v>384</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="D8" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="E8" s="3">
+      <c r="E8" s="2">
         <v>0</v>
       </c>
-      <c r="F8" s="3" t="s">
+      <c r="F8" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="G8" s="3">
-        <v>1</v>
-      </c>
-      <c r="H8" s="3" t="s">
+      <c r="G8" s="2">
+        <v>1</v>
+      </c>
+      <c r="H8" s="2" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A9" s="3">
+      <c r="A9" s="2">
         <v>4</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B9" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C9" s="3">
+      <c r="C9" s="2">
         <v>384</v>
       </c>
-      <c r="D9" s="3" t="s">
+      <c r="D9" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="E9" s="3">
+      <c r="E9" s="2">
         <v>0</v>
       </c>
-      <c r="F9" s="3" t="s">
+      <c r="F9" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="G9" s="3">
-        <v>1</v>
-      </c>
-      <c r="H9" s="3" t="s">
+      <c r="G9" s="2">
+        <v>1</v>
+      </c>
+      <c r="H9" s="2" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A10" s="3">
+      <c r="A10" s="2">
         <v>5</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B10" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C10" s="3">
+      <c r="C10" s="2">
         <v>256</v>
       </c>
-      <c r="D10" s="3" t="s">
+      <c r="D10" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="E10" s="3">
+      <c r="E10" s="2">
         <v>0</v>
       </c>
-      <c r="F10" s="3" t="s">
+      <c r="F10" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="G10" s="3">
-        <v>1</v>
-      </c>
-      <c r="H10" s="3" t="s">
+      <c r="G10" s="2">
+        <v>1</v>
+      </c>
+      <c r="H10" s="2" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A11" s="3"/>
-      <c r="B11" s="3" t="s">
+      <c r="A11" s="2"/>
+      <c r="B11" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C11" s="3">
+      <c r="C11" s="2">
         <v>256</v>
       </c>
-      <c r="D11" s="3" t="s">
+      <c r="D11" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="E11" s="3">
+      <c r="E11" s="2">
         <v>0</v>
       </c>
-      <c r="F11" s="3" t="s">
+      <c r="F11" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="G11" s="3">
+      <c r="G11" s="2">
         <v>2</v>
       </c>
-      <c r="H11" s="3" t="s">
+      <c r="H11" s="2" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A12" s="3">
+      <c r="A12" s="2">
         <v>6</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="B12" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C12" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D12" s="3">
+      <c r="C12" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D12" s="2">
         <v>9216</v>
       </c>
-      <c r="E12" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="F12" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="G12" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="H12" s="3" t="s">
+      <c r="E12" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H12" s="2" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A13" s="3">
+      <c r="A13" s="2">
         <v>7</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="B13" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C13" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D13" s="3">
+      <c r="C13" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D13" s="2">
         <v>4096</v>
       </c>
-      <c r="E13" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="F13" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="G13" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="H13" s="3" t="s">
+      <c r="E13" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G13" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H13" s="2" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A14" s="3" t="s">
+      <c r="A14" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B14" s="3" t="s">
+      <c r="B14" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C14" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D14" s="3">
+      <c r="C14" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D14" s="2">
         <v>1000</v>
       </c>
-      <c r="E14" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="F14" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="G14" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="H14" s="3" t="s">
+      <c r="E14" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G14" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H14" s="2" t="s">
         <v>23</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="7">
+    <mergeCell ref="H1:H2"/>
+    <mergeCell ref="E1:E2"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="C1:C2"/>
     <mergeCell ref="D1:D2"/>
     <mergeCell ref="F1:F2"/>
     <mergeCell ref="G1:G2"/>
-    <mergeCell ref="H1:H2"/>
-    <mergeCell ref="E1:E2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -953,10 +953,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{578F8903-D2E9-4756-A4BF-916B46974A54}">
-  <dimension ref="A1:J12"/>
+  <dimension ref="A1:J13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -967,52 +967,52 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="7" t="s">
+      <c r="B1" s="12"/>
+      <c r="C1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="D1" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="11" t="s">
+      <c r="E1" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="F1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="G1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="H1" s="7" t="s">
+      <c r="H1" s="4" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A2" s="12" t="s">
+      <c r="A2" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="3">
-        <v>1</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="H2" s="4" t="s">
+      <c r="C2" s="2">
+        <v>1</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H2" s="3" t="s">
         <v>12</v>
       </c>
       <c r="J2" t="s">
@@ -1020,263 +1020,289 @@
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C3" s="2">
+        <v>32</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E3" s="2">
+        <v>0</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G3" s="2">
+        <v>2</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A4" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B4" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C4" s="2">
+        <v>32</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E4" s="2">
+        <v>0</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G4" s="2">
+        <v>2</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A5" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C5" s="2">
+        <v>64</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="E5" s="2">
+        <v>1</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G5" s="2">
+        <v>1</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A6" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C6" s="2">
+        <v>64</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="E6" s="2">
+        <v>1</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G6" s="2">
+        <v>1</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A7" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C7" s="2">
+        <v>64</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="E7" s="2">
+        <v>1</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G7" s="2">
+        <v>1</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A8" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C8" s="2">
+        <v>64</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E8" s="2">
+        <v>0</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G8" s="2">
+        <v>2</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A9" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C9" s="3">
+        <v>64</v>
+      </c>
+      <c r="D9" s="2">
+        <v>3136</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A10" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B10" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="C3" s="3">
-        <v>32</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="E3" s="3">
-        <v>0</v>
-      </c>
-      <c r="F3" s="3" t="s">
+      <c r="C10" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D10" s="2">
+        <v>3136</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A11" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D11" s="2">
+        <v>512</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A12" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D12" s="2">
+        <v>64</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A13" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="G3" s="3">
-        <v>2</v>
-      </c>
-      <c r="H3" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A4" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="C4" s="3">
-        <v>32</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="E4" s="3">
-        <v>0</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="G4" s="3">
-        <v>2</v>
-      </c>
-      <c r="H4" s="4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A5" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="B5" s="3" t="s">
+      <c r="B13" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="C5" s="3">
-        <v>64</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="E5" s="3">
-        <v>1</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="G5" s="3">
-        <v>1</v>
-      </c>
-      <c r="H5" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A6" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="C6" s="3">
-        <v>64</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="E6" s="3">
-        <v>1</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="G6" s="3">
-        <v>1</v>
-      </c>
-      <c r="H6" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A7" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="C7" s="3">
-        <v>64</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="E7" s="3">
-        <v>1</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="G7" s="3">
-        <v>1</v>
-      </c>
-      <c r="H7" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A8" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="C8" s="3">
-        <v>64</v>
-      </c>
-      <c r="D8" s="3" t="s">
+      <c r="C13" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D13" s="2">
+        <v>1</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G13" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H13" s="2" t="s">
         <v>45</v>
-      </c>
-      <c r="E8" s="3">
-        <v>0</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="G8" s="3">
-        <v>2</v>
-      </c>
-      <c r="H8" s="4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A9" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D9" s="3">
-        <v>3136</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="F9" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="G9" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="H9" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A10" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D10" s="3">
-        <v>512</v>
-      </c>
-      <c r="E10" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="F10" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="G10" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="H10" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A11" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D11" s="3">
-        <v>64</v>
-      </c>
-      <c r="E11" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="F11" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="G11" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="H11" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A12" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D12" s="3">
-        <v>1</v>
-      </c>
-      <c r="E12" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="F12" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="G12" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="H12" s="3" t="s">
-        <v>41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>